<commit_message>
Add new tables and figures for the 10% sample
</commit_message>
<xml_diff>
--- a/03_Tables/muestra_10porciento/SelfUpdate_twfe_wage_heterogeneity.xlsx
+++ b/03_Tables/muestra_10porciento/SelfUpdate_twfe_wage_heterogeneity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcomedina/ITAM Seira Research Dropbox/Marco Alejandro Medina/imss_rpci/03_Tables/muestra_10porciento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78A6CBE-DFA8-5945-BF29-9B31555B7082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154D0E31-D2E4-ED49-9D35-E2684DC2ED36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="2" xr2:uid="{5F2EF16D-A70A-3F40-9EFD-AA737EECFF16}"/>
   </bookViews>
@@ -17,6 +17,12 @@
     <sheet name="twfe_wage_hetero_firm_char" sheetId="7" r:id="rId2"/>
     <sheet name="twfe_wage_hetero_firm_size" sheetId="8" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,6 +42,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
@@ -148,10 +176,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="\(0.000\)"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="\(0.000\)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="\(0.00\)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -244,7 +274,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,14 +293,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -285,19 +315,34 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -317,6 +362,855 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="twfe_sal_cierre_heterogeneity"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>7.6***</v>
+          </cell>
+          <cell r="C3">
+            <v>0.4</v>
+          </cell>
+          <cell r="D3">
+            <v>-0.3</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>4.5**</v>
+          </cell>
+          <cell r="F3">
+            <v>0.4</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>17.1***</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>3.7***</v>
+          </cell>
+          <cell r="I3" t="str">
+            <v>7.9***</v>
+          </cell>
+          <cell r="J3" t="str">
+            <v>3.4**</v>
+          </cell>
+          <cell r="K3" t="str">
+            <v>9.1***</v>
+          </cell>
+          <cell r="L3" t="str">
+            <v>5.0***</v>
+          </cell>
+          <cell r="M3" t="str">
+            <v>3.6***</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>0.98</v>
+          </cell>
+          <cell r="C4">
+            <v>0.92</v>
+          </cell>
+          <cell r="D4">
+            <v>1.4</v>
+          </cell>
+          <cell r="E4">
+            <v>1.79</v>
+          </cell>
+          <cell r="F4">
+            <v>1.26</v>
+          </cell>
+          <cell r="G4">
+            <v>2.95</v>
+          </cell>
+          <cell r="H4">
+            <v>1.4</v>
+          </cell>
+          <cell r="I4">
+            <v>2.82</v>
+          </cell>
+          <cell r="J4">
+            <v>1.56</v>
+          </cell>
+          <cell r="K4">
+            <v>1.59</v>
+          </cell>
+          <cell r="L4">
+            <v>0.89</v>
+          </cell>
+          <cell r="M4">
+            <v>1.32</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>469.8***</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>412.1***</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>524.1***</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>398.0***</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>464.4***</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>312.0***</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>386.3***</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>481.7***</v>
+          </cell>
+          <cell r="J5" t="str">
+            <v>454.0***</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>572.8***</v>
+          </cell>
+          <cell r="L5" t="str">
+            <v>360.0***</v>
+          </cell>
+          <cell r="M5" t="str">
+            <v>566.1***</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0.01</v>
+          </cell>
+          <cell r="C6">
+            <v>0.01</v>
+          </cell>
+          <cell r="D6">
+            <v>0.02</v>
+          </cell>
+          <cell r="E6">
+            <v>0.02</v>
+          </cell>
+          <cell r="F6">
+            <v>0.01</v>
+          </cell>
+          <cell r="G6">
+            <v>0.03</v>
+          </cell>
+          <cell r="H6">
+            <v>0.02</v>
+          </cell>
+          <cell r="I6">
+            <v>0.03</v>
+          </cell>
+          <cell r="J6">
+            <v>0.02</v>
+          </cell>
+          <cell r="K6">
+            <v>0.02</v>
+          </cell>
+          <cell r="L6">
+            <v>0.01</v>
+          </cell>
+          <cell r="M6">
+            <v>0.02</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>36408980</v>
+          </cell>
+          <cell r="C7">
+            <v>22676833</v>
+          </cell>
+          <cell r="D7">
+            <v>15323763</v>
+          </cell>
+          <cell r="E7">
+            <v>8282504</v>
+          </cell>
+          <cell r="F7">
+            <v>16368078</v>
+          </cell>
+          <cell r="G7">
+            <v>4367222</v>
+          </cell>
+          <cell r="H7">
+            <v>12051628</v>
+          </cell>
+          <cell r="I7">
+            <v>3572215</v>
+          </cell>
+          <cell r="J7">
+            <v>13451793</v>
+          </cell>
+          <cell r="K7">
+            <v>6561557</v>
+          </cell>
+          <cell r="L7">
+            <v>30128902</v>
+          </cell>
+          <cell r="M7">
+            <v>15597960</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>469.8</v>
+          </cell>
+          <cell r="C8">
+            <v>412.1</v>
+          </cell>
+          <cell r="D8">
+            <v>524.1</v>
+          </cell>
+          <cell r="E8">
+            <v>398.1</v>
+          </cell>
+          <cell r="F8">
+            <v>464.4</v>
+          </cell>
+          <cell r="G8">
+            <v>312.2</v>
+          </cell>
+          <cell r="H8">
+            <v>386.4</v>
+          </cell>
+          <cell r="I8">
+            <v>481.8</v>
+          </cell>
+          <cell r="J8">
+            <v>454.1</v>
+          </cell>
+          <cell r="K8">
+            <v>572.9</v>
+          </cell>
+          <cell r="L8">
+            <v>360.1</v>
+          </cell>
+          <cell r="M8">
+            <v>566.1</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>1536994</v>
+          </cell>
+          <cell r="C9">
+            <v>949276</v>
+          </cell>
+          <cell r="D9">
+            <v>633118</v>
+          </cell>
+          <cell r="E9">
+            <v>411987</v>
+          </cell>
+          <cell r="F9">
+            <v>653573</v>
+          </cell>
+          <cell r="G9">
+            <v>237124</v>
+          </cell>
+          <cell r="H9">
+            <v>494585</v>
+          </cell>
+          <cell r="I9">
+            <v>142759</v>
+          </cell>
+          <cell r="J9">
+            <v>581209</v>
+          </cell>
+          <cell r="K9">
+            <v>240476</v>
+          </cell>
+          <cell r="L9">
+            <v>1591091</v>
+          </cell>
+          <cell r="M9">
+            <v>619002</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>421422</v>
+          </cell>
+          <cell r="C10">
+            <v>283428</v>
+          </cell>
+          <cell r="D10">
+            <v>125402</v>
+          </cell>
+          <cell r="E10">
+            <v>145157</v>
+          </cell>
+          <cell r="F10">
+            <v>139210</v>
+          </cell>
+          <cell r="G10">
+            <v>133480</v>
+          </cell>
+          <cell r="H10">
+            <v>186241</v>
+          </cell>
+          <cell r="I10">
+            <v>63206</v>
+          </cell>
+          <cell r="J10">
+            <v>213668</v>
+          </cell>
+          <cell r="K10">
+            <v>48247</v>
+          </cell>
+          <cell r="L10">
+            <v>527133</v>
+          </cell>
+          <cell r="M10">
+            <v>78339</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="twfe_log_sal_cierre_heterogenei"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>0.02***</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="D3">
+            <v>0</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="F3">
+            <v>0</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>0.04***</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="I3" t="str">
+            <v>0.02***</v>
+          </cell>
+          <cell r="J3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="K3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="L3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="M3" t="str">
+            <v>0.01***</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>2E-3</v>
+          </cell>
+          <cell r="C4">
+            <v>2E-3</v>
+          </cell>
+          <cell r="D4">
+            <v>2E-3</v>
+          </cell>
+          <cell r="E4">
+            <v>3.0000000000000001E-3</v>
+          </cell>
+          <cell r="F4">
+            <v>2E-3</v>
+          </cell>
+          <cell r="G4">
+            <v>5.0000000000000001E-3</v>
+          </cell>
+          <cell r="H4">
+            <v>3.0000000000000001E-3</v>
+          </cell>
+          <cell r="I4">
+            <v>5.0000000000000001E-3</v>
+          </cell>
+          <cell r="J4">
+            <v>3.0000000000000001E-3</v>
+          </cell>
+          <cell r="K4">
+            <v>3.0000000000000001E-3</v>
+          </cell>
+          <cell r="L4">
+            <v>2E-3</v>
+          </cell>
+          <cell r="M4">
+            <v>2E-3</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>5.83***</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>5.74***</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>5.96***</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>5.74***</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>5.88***</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>5.50***</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>5.69***</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>5.87***</v>
+          </cell>
+          <cell r="J5" t="str">
+            <v>5.73***</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>6.09***</v>
+          </cell>
+          <cell r="L5" t="str">
+            <v>5.59***</v>
+          </cell>
+          <cell r="M5" t="str">
+            <v>6.07***</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0</v>
+          </cell>
+          <cell r="C6">
+            <v>0</v>
+          </cell>
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+          <cell r="E6">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>0</v>
+          </cell>
+          <cell r="G6">
+            <v>0</v>
+          </cell>
+          <cell r="H6">
+            <v>0</v>
+          </cell>
+          <cell r="I6">
+            <v>0</v>
+          </cell>
+          <cell r="J6">
+            <v>0</v>
+          </cell>
+          <cell r="K6">
+            <v>0</v>
+          </cell>
+          <cell r="L6">
+            <v>0</v>
+          </cell>
+          <cell r="M6">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>5.83</v>
+          </cell>
+          <cell r="C8">
+            <v>5.74</v>
+          </cell>
+          <cell r="D8">
+            <v>5.96</v>
+          </cell>
+          <cell r="E8">
+            <v>5.74</v>
+          </cell>
+          <cell r="F8">
+            <v>5.88</v>
+          </cell>
+          <cell r="G8">
+            <v>5.5</v>
+          </cell>
+          <cell r="H8">
+            <v>5.69</v>
+          </cell>
+          <cell r="I8">
+            <v>5.87</v>
+          </cell>
+          <cell r="J8">
+            <v>5.73</v>
+          </cell>
+          <cell r="K8">
+            <v>6.09</v>
+          </cell>
+          <cell r="L8">
+            <v>5.59</v>
+          </cell>
+          <cell r="M8">
+            <v>6.07</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="twfe_sal_cierre_heterogeneity_f"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>11.2**</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>12.3***</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>8.1***</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>4.6***</v>
+          </cell>
+          <cell r="F3">
+            <v>3.4</v>
+          </cell>
+          <cell r="G3">
+            <v>-1.5</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>3.6***</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>4.8600000000000003</v>
+          </cell>
+          <cell r="C4">
+            <v>2.85</v>
+          </cell>
+          <cell r="D4">
+            <v>1.48</v>
+          </cell>
+          <cell r="E4">
+            <v>1.52</v>
+          </cell>
+          <cell r="F4">
+            <v>2.08</v>
+          </cell>
+          <cell r="G4">
+            <v>2.14</v>
+          </cell>
+          <cell r="H4">
+            <v>1.32</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>224.0***</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>235.1***</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>325.7***</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>436.6***</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>492.1***</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>507.2***</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>566.1***</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0.04</v>
+          </cell>
+          <cell r="C6">
+            <v>0.03</v>
+          </cell>
+          <cell r="D6">
+            <v>0.02</v>
+          </cell>
+          <cell r="E6">
+            <v>0.02</v>
+          </cell>
+          <cell r="F6">
+            <v>0.03</v>
+          </cell>
+          <cell r="G6">
+            <v>0.02</v>
+          </cell>
+          <cell r="H6">
+            <v>0.02</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>750198</v>
+          </cell>
+          <cell r="C7">
+            <v>3300834</v>
+          </cell>
+          <cell r="D7">
+            <v>12373430</v>
+          </cell>
+          <cell r="E7">
+            <v>13797897</v>
+          </cell>
+          <cell r="F7">
+            <v>6822982</v>
+          </cell>
+          <cell r="G7">
+            <v>6422833</v>
+          </cell>
+          <cell r="H7">
+            <v>15597960</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>224.1</v>
+          </cell>
+          <cell r="C8">
+            <v>235.2</v>
+          </cell>
+          <cell r="D8">
+            <v>325.8</v>
+          </cell>
+          <cell r="E8">
+            <v>436.7</v>
+          </cell>
+          <cell r="F8">
+            <v>492.1</v>
+          </cell>
+          <cell r="G8">
+            <v>507.2</v>
+          </cell>
+          <cell r="H8">
+            <v>566.1</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>31993</v>
+          </cell>
+          <cell r="C9">
+            <v>145267</v>
+          </cell>
+          <cell r="D9">
+            <v>545340</v>
+          </cell>
+          <cell r="E9">
+            <v>590009</v>
+          </cell>
+          <cell r="F9">
+            <v>286824</v>
+          </cell>
+          <cell r="G9">
+            <v>266509</v>
+          </cell>
+          <cell r="H9">
+            <v>619002</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>40609</v>
+          </cell>
+          <cell r="C10">
+            <v>172140</v>
+          </cell>
+          <cell r="D10">
+            <v>317794</v>
+          </cell>
+          <cell r="E10">
+            <v>149345</v>
+          </cell>
+          <cell r="F10">
+            <v>76158</v>
+          </cell>
+          <cell r="G10">
+            <v>61901</v>
+          </cell>
+          <cell r="H10">
+            <v>78339</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="twfe_log_sal_cierre_heterogenei"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>0.03***</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>0.03***</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>0.02***</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>0.01***</v>
+          </cell>
+          <cell r="G3">
+            <v>0</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>0.01***</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>1.0999999999999999E-2</v>
+          </cell>
+          <cell r="C4">
+            <v>5.0000000000000001E-3</v>
+          </cell>
+          <cell r="D4">
+            <v>3.0000000000000001E-3</v>
+          </cell>
+          <cell r="E4">
+            <v>3.0000000000000001E-3</v>
+          </cell>
+          <cell r="F4">
+            <v>4.0000000000000001E-3</v>
+          </cell>
+          <cell r="G4">
+            <v>4.0000000000000001E-3</v>
+          </cell>
+          <cell r="H4">
+            <v>2E-3</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>5.22***</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>5.28***</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>5.52***</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>5.77***</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>5.89***</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>5.94***</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>6.07***</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0</v>
+          </cell>
+          <cell r="C6">
+            <v>0</v>
+          </cell>
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+          <cell r="E6">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>0</v>
+          </cell>
+          <cell r="G6">
+            <v>0</v>
+          </cell>
+          <cell r="H6">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>5.22</v>
+          </cell>
+          <cell r="C8">
+            <v>5.28</v>
+          </cell>
+          <cell r="D8">
+            <v>5.52</v>
+          </cell>
+          <cell r="E8">
+            <v>5.77</v>
+          </cell>
+          <cell r="F8">
+            <v>5.89</v>
+          </cell>
+          <cell r="G8">
+            <v>5.94</v>
+          </cell>
+          <cell r="H8">
+            <v>6.07</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,7 +1513,7 @@
   <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F19" sqref="B3:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,139 +1563,249 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="5" t="str" cm="1">
+        <f t="array" ref="C6:F9">[1]twfe_sal_cierre_heterogeneity!$B$3:$E$6</f>
+        <v>7.6***</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="E6" s="17">
+        <v>-0.3</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <v>4.5**</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="C7" s="11">
+        <v>0.98</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.92</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1.79</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="5" t="str">
+        <v>469.8***</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <v>412.1***</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <v>524.1***</v>
+      </c>
+      <c r="F8" s="5" t="str">
+        <v>398.0***</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="C9" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="18" cm="1">
+        <f t="array" ref="C10:F10">[1]twfe_sal_cierre_heterogeneity!$B$8:$E$8</f>
+        <v>469.8</v>
+      </c>
+      <c r="D10" s="18">
+        <v>412.1</v>
+      </c>
+      <c r="E10" s="18">
+        <v>524.1</v>
+      </c>
+      <c r="F10" s="18">
+        <v>398.1</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="5" t="str" cm="1">
+        <f t="array" ref="C12:F15">[2]twfe_log_sal_cierre_heterogenei!$B$3:$E$6</f>
+        <v>0.02***</v>
+      </c>
+      <c r="D12" s="21" t="str">
+        <v>0.01***</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="str">
+        <v>0.01***</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="C13" s="11">
+        <v>2E-3</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2E-3</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2E-3</v>
+      </c>
+      <c r="F13" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="C14" s="5" t="str">
+        <v>5.83***</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <v>5.74***</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <v>5.96***</v>
+      </c>
+      <c r="F14" s="5" t="str">
+        <v>5.74***</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="C16" s="5" cm="1">
+        <f t="array" ref="C16:F16">[2]twfe_log_sal_cierre_heterogenei!$B$8:$E$8</f>
+        <v>5.83</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5.74</v>
+      </c>
+      <c r="E16" s="5">
+        <v>5.96</v>
+      </c>
+      <c r="F16" s="5">
+        <v>5.74</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="C17" s="10" cm="1">
+        <f t="array" ref="C17:F17">[1]twfe_sal_cierre_heterogeneity!$B$7:$E$7</f>
+        <v>36408980</v>
+      </c>
+      <c r="D17" s="10">
+        <v>22676833</v>
+      </c>
+      <c r="E17" s="10">
+        <v>15323763</v>
+      </c>
+      <c r="F17" s="10">
+        <v>8282504</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="12" cm="1">
+        <f t="array" ref="C18:F19">[1]twfe_sal_cierre_heterogeneity!$B$9:$E$10</f>
+        <v>1536994</v>
+      </c>
+      <c r="D18" s="13">
+        <v>949276</v>
+      </c>
+      <c r="E18" s="13">
+        <v>633118</v>
+      </c>
+      <c r="F18" s="12">
+        <v>411987</v>
+      </c>
     </row>
     <row r="19" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="C19" s="9">
+        <v>421422</v>
+      </c>
+      <c r="D19" s="9">
+        <v>283428</v>
+      </c>
+      <c r="E19" s="9">
+        <v>125402</v>
+      </c>
+      <c r="F19" s="9">
+        <v>145157</v>
+      </c>
     </row>
     <row r="20" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
@@ -831,7 +1835,7 @@
   <dimension ref="B2:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="B3" sqref="B3:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,200 +1913,414 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="C6" s="5" cm="1">
+        <f t="array" ref="C6:J9">[1]twfe_sal_cierre_heterogeneity!$F$3:$M$6</f>
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <v>17.1***</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <v>3.7***</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <v>7.9***</v>
+      </c>
+      <c r="G6" s="5" t="str">
+        <v>3.4**</v>
+      </c>
+      <c r="H6" s="5" t="str">
+        <v>9.1***</v>
+      </c>
+      <c r="I6" s="5" t="str">
+        <v>5.0***</v>
+      </c>
+      <c r="J6" s="5" t="str">
+        <v>3.6***</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="C7" s="11">
+        <v>1.26</v>
+      </c>
+      <c r="D7" s="11">
+        <v>2.95</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="F7" s="11">
+        <v>2.82</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1.56</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1.59</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.89</v>
+      </c>
+      <c r="J7" s="11">
+        <v>1.32</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="C8" s="5" t="str">
+        <v>464.4***</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <v>312.0***</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <v>386.3***</v>
+      </c>
+      <c r="F8" s="5" t="str">
+        <v>481.7***</v>
+      </c>
+      <c r="G8" s="5" t="str">
+        <v>454.0***</v>
+      </c>
+      <c r="H8" s="5" t="str">
+        <v>572.8***</v>
+      </c>
+      <c r="I8" s="5" t="str">
+        <v>360.0***</v>
+      </c>
+      <c r="J8" s="5" t="str">
+        <v>566.1***</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="C9" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="C10" s="5" cm="1">
+        <f t="array" ref="C10:J10">[1]twfe_sal_cierre_heterogeneity!$F$8:$M$8</f>
+        <v>464.4</v>
+      </c>
+      <c r="D10" s="5">
+        <v>312.2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>386.4</v>
+      </c>
+      <c r="F10" s="5">
+        <v>481.8</v>
+      </c>
+      <c r="G10" s="5">
+        <v>454.1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>572.9</v>
+      </c>
+      <c r="I10" s="5">
+        <v>360.1</v>
+      </c>
+      <c r="J10" s="5">
+        <v>566.1</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="C12" s="25" cm="1">
+        <f t="array" ref="C12:J15">[2]twfe_log_sal_cierre_heterogenei!$F$3:$M$6</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="14" t="str">
+        <v>0.04***</v>
+      </c>
+      <c r="E12" s="14" t="str">
+        <v>0.01***</v>
+      </c>
+      <c r="F12" s="14" t="str">
+        <v>0.02***</v>
+      </c>
+      <c r="G12" s="14" t="str">
+        <v>0.01***</v>
+      </c>
+      <c r="H12" s="14" t="str">
+        <v>0.01***</v>
+      </c>
+      <c r="I12" s="14" t="str">
+        <v>0.01***</v>
+      </c>
+      <c r="J12" s="14" t="str">
+        <v>0.01***</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="C13" s="11">
+        <v>2E-3</v>
+      </c>
+      <c r="D13" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E13" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F13" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G13" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H13" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I13" s="11">
+        <v>2E-3</v>
+      </c>
+      <c r="J13" s="11">
+        <v>2E-3</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="C14" s="5" t="str">
+        <v>5.88***</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <v>5.50***</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <v>5.69***</v>
+      </c>
+      <c r="F14" s="5" t="str">
+        <v>5.87***</v>
+      </c>
+      <c r="G14" s="5" t="str">
+        <v>5.73***</v>
+      </c>
+      <c r="H14" s="5" t="str">
+        <v>6.09***</v>
+      </c>
+      <c r="I14" s="5" t="str">
+        <v>5.59***</v>
+      </c>
+      <c r="J14" s="5" t="str">
+        <v>6.07***</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="C16" s="1" cm="1">
+        <f t="array" ref="C16:J16">[2]twfe_log_sal_cierre_heterogenei!$F$8:$M$8</f>
+        <v>5.88</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5.69</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5.87</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5.73</v>
+      </c>
+      <c r="H16" s="1">
+        <v>6.09</v>
+      </c>
+      <c r="I16" s="1">
+        <v>5.59</v>
+      </c>
+      <c r="J16" s="1">
+        <v>6.07</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="C17" s="10" cm="1">
+        <f t="array" ref="C17:J17">[1]twfe_sal_cierre_heterogeneity!$F$7:$M$7</f>
+        <v>16368078</v>
+      </c>
+      <c r="D17" s="10">
+        <v>4367222</v>
+      </c>
+      <c r="E17" s="10">
+        <v>12051628</v>
+      </c>
+      <c r="F17" s="10">
+        <v>3572215</v>
+      </c>
+      <c r="G17" s="10">
+        <v>13451793</v>
+      </c>
+      <c r="H17" s="10">
+        <v>6561557</v>
+      </c>
+      <c r="I17" s="10">
+        <v>30128902</v>
+      </c>
+      <c r="J17" s="10">
+        <v>15597960</v>
+      </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="C18" s="12" cm="1">
+        <f t="array" ref="C18:J19">[1]twfe_sal_cierre_heterogeneity!$F$9:$M$10</f>
+        <v>653573</v>
+      </c>
+      <c r="D18" s="13">
+        <v>237124</v>
+      </c>
+      <c r="E18" s="13">
+        <v>494585</v>
+      </c>
+      <c r="F18" s="13">
+        <v>142759</v>
+      </c>
+      <c r="G18" s="13">
+        <v>581209</v>
+      </c>
+      <c r="H18" s="13">
+        <v>240476</v>
+      </c>
+      <c r="I18" s="13">
+        <v>1591091</v>
+      </c>
+      <c r="J18" s="13">
+        <v>619002</v>
+      </c>
     </row>
     <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="C19" s="9">
+        <v>139210</v>
+      </c>
+      <c r="D19" s="9">
+        <v>133480</v>
+      </c>
+      <c r="E19" s="9">
+        <v>186241</v>
+      </c>
+      <c r="F19" s="9">
+        <v>63206</v>
+      </c>
+      <c r="G19" s="9">
+        <v>213668</v>
+      </c>
+      <c r="H19" s="9">
+        <v>48247</v>
+      </c>
+      <c r="I19" s="9">
+        <v>527133</v>
+      </c>
+      <c r="J19" s="9">
+        <v>78339</v>
+      </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
@@ -1129,7 +2347,7 @@
   <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H26" sqref="H26:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1159,7 +2377,7 @@
       <c r="D3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1207,15 +2425,15 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1223,13 +2441,28 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="C6" s="5" t="str" cm="1">
+        <f t="array" ref="C6:I9">[3]twfe_sal_cierre_heterogeneity_f!$B$3:$H$6</f>
+        <v>11.2**</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <v>12.3***</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <v>8.1***</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <v>4.6***</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="H6" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="I6" s="5" t="str">
+        <v>3.6***</v>
+      </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1237,13 +2470,27 @@
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="C7" s="19">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="D7" s="19">
+        <v>2.85</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1.48</v>
+      </c>
+      <c r="F7" s="19">
+        <v>1.52</v>
+      </c>
+      <c r="G7" s="19">
+        <v>2.08</v>
+      </c>
+      <c r="H7" s="19">
+        <v>2.14</v>
+      </c>
+      <c r="I7" s="19">
+        <v>1.32</v>
+      </c>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1251,25 +2498,53 @@
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="C8" s="5" t="str">
+        <v>224.0***</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <v>235.1***</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <v>325.7***</v>
+      </c>
+      <c r="F8" s="5" t="str">
+        <v>436.6***</v>
+      </c>
+      <c r="G8" s="5" t="str">
+        <v>492.1***</v>
+      </c>
+      <c r="H8" s="5" t="str">
+        <v>507.2***</v>
+      </c>
+      <c r="I8" s="5" t="str">
+        <v>566.1***</v>
+      </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="C9" s="19">
+        <v>0.04</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0.03</v>
+      </c>
+      <c r="E9" s="19">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.02</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0.03</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.02</v>
+      </c>
+      <c r="I9" s="19">
+        <v>0.02</v>
+      </c>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1277,13 +2552,28 @@
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="C10" s="20" cm="1">
+        <f t="array" ref="C10:I10">[3]twfe_sal_cierre_heterogeneity_f!$B$8:$H$8</f>
+        <v>224.1</v>
+      </c>
+      <c r="D10" s="20">
+        <v>235.2</v>
+      </c>
+      <c r="E10" s="20">
+        <v>325.8</v>
+      </c>
+      <c r="F10" s="20">
+        <v>436.7</v>
+      </c>
+      <c r="G10" s="20">
+        <v>492.1</v>
+      </c>
+      <c r="H10" s="20">
+        <v>507.2</v>
+      </c>
+      <c r="I10" s="20">
+        <v>566.1</v>
+      </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1291,15 +2581,15 @@
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1307,13 +2597,28 @@
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="C12" s="5" t="str" cm="1">
+        <f t="array" ref="C12:I15">[4]twfe_log_sal_cierre_heterogenei!$B$3:$H$6</f>
+        <v>0.03***</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <v>0.03***</v>
+      </c>
+      <c r="E12" s="5" t="str">
+        <v>0.02***</v>
+      </c>
+      <c r="F12" s="5" t="str">
+        <v>0.01***</v>
+      </c>
+      <c r="G12" s="5" t="str">
+        <v>0.01***</v>
+      </c>
+      <c r="H12" s="21">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="str">
+        <v>0.01***</v>
+      </c>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1321,13 +2626,27 @@
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="C13" s="11">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D13" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E13" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F13" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G13" s="11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H13" s="11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I13" s="11">
+        <v>2E-3</v>
+      </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1335,25 +2654,53 @@
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="C14" s="5" t="str">
+        <v>5.22***</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <v>5.28***</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <v>5.52***</v>
+      </c>
+      <c r="F14" s="5" t="str">
+        <v>5.77***</v>
+      </c>
+      <c r="G14" s="5" t="str">
+        <v>5.89***</v>
+      </c>
+      <c r="H14" s="5" t="str">
+        <v>5.94***</v>
+      </c>
+      <c r="I14" s="5" t="str">
+        <v>6.07***</v>
+      </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1361,13 +2708,28 @@
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="C16" s="18" cm="1">
+        <f t="array" ref="C16:I16">[4]twfe_log_sal_cierre_heterogenei!$B$8:$H$8</f>
+        <v>5.22</v>
+      </c>
+      <c r="D16" s="18">
+        <v>5.28</v>
+      </c>
+      <c r="E16" s="18">
+        <v>5.52</v>
+      </c>
+      <c r="F16" s="18">
+        <v>5.77</v>
+      </c>
+      <c r="G16" s="18">
+        <v>5.89</v>
+      </c>
+      <c r="H16" s="18">
+        <v>5.94</v>
+      </c>
+      <c r="I16" s="18">
+        <v>6.07</v>
+      </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1375,13 +2737,28 @@
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="C17" s="12" cm="1">
+        <f t="array" ref="C17:I17">[3]twfe_sal_cierre_heterogeneity_f!$B$7:$H$7</f>
+        <v>750198</v>
+      </c>
+      <c r="D17" s="12">
+        <v>3300834</v>
+      </c>
+      <c r="E17" s="12">
+        <v>12373430</v>
+      </c>
+      <c r="F17" s="12">
+        <v>13797897</v>
+      </c>
+      <c r="G17" s="12">
+        <v>6822982</v>
+      </c>
+      <c r="H17" s="12">
+        <v>6422833</v>
+      </c>
+      <c r="I17" s="12">
+        <v>15597960</v>
+      </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1389,13 +2766,28 @@
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="C18" s="12" cm="1">
+        <f t="array" ref="C18:I19">[3]twfe_sal_cierre_heterogeneity_f!$B$9:$H$10</f>
+        <v>31993</v>
+      </c>
+      <c r="D18" s="13">
+        <v>145267</v>
+      </c>
+      <c r="E18" s="13">
+        <v>545340</v>
+      </c>
+      <c r="F18" s="13">
+        <v>590009</v>
+      </c>
+      <c r="G18" s="13">
+        <v>286824</v>
+      </c>
+      <c r="H18" s="13">
+        <v>266509</v>
+      </c>
+      <c r="I18" s="13">
+        <v>619002</v>
+      </c>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1403,13 +2795,27 @@
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="C19" s="9">
+        <v>40609</v>
+      </c>
+      <c r="D19" s="9">
+        <v>172140</v>
+      </c>
+      <c r="E19" s="9">
+        <v>317794</v>
+      </c>
+      <c r="F19" s="9">
+        <v>149345</v>
+      </c>
+      <c r="G19" s="9">
+        <v>76158</v>
+      </c>
+      <c r="H19" s="9">
+        <v>61901</v>
+      </c>
+      <c r="I19" s="9">
+        <v>78339</v>
+      </c>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>